<commit_message>
update pydantic and excel sheets after merging
</commit_message>
<xml_diff>
--- a/excel_sheets/Timeseries_metadata.xlsx
+++ b/excel_sheets/Timeseries_metadata.xlsx
@@ -507,7 +507,7 @@
       <c r="B1" s="2" t="n"/>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>timeseries type metadata version 20240812.1</t>
+          <t>timeseries type metadata version 20240905.1</t>
         </is>
       </c>
       <c r="D1" s="2" t="n"/>
@@ -3304,7 +3304,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD295"/>
+  <dimension ref="A1:AD296"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6032,7 +6032,7 @@
           <t>uri</t>
         </is>
       </c>
-      <c r="C77" s="6" t="inlineStr"/>
+      <c r="C77" s="6" t="n"/>
       <c r="D77" s="6" t="n"/>
       <c r="E77" s="6" t="n"/>
       <c r="F77" s="6" t="n"/>
@@ -6208,7 +6208,7 @@
           <t>uri</t>
         </is>
       </c>
-      <c r="C82" s="6" t="inlineStr"/>
+      <c r="C82" s="6" t="n"/>
       <c r="D82" s="6" t="n"/>
       <c r="E82" s="6" t="n"/>
       <c r="F82" s="6" t="n"/>
@@ -6808,7 +6808,7 @@
           <t>uri</t>
         </is>
       </c>
-      <c r="C99" s="6" t="inlineStr"/>
+      <c r="C99" s="6" t="n"/>
       <c r="D99" s="6" t="n"/>
       <c r="E99" s="6" t="n"/>
       <c r="F99" s="6" t="n"/>
@@ -6984,7 +6984,7 @@
           <t>uri</t>
         </is>
       </c>
-      <c r="C104" s="6" t="inlineStr"/>
+      <c r="C104" s="6" t="n"/>
       <c r="D104" s="6" t="n"/>
       <c r="E104" s="6" t="n"/>
       <c r="F104" s="6" t="n"/>
@@ -7160,7 +7160,7 @@
           <t>uri</t>
         </is>
       </c>
-      <c r="C109" s="6" t="inlineStr"/>
+      <c r="C109" s="6" t="n"/>
       <c r="D109" s="6" t="n"/>
       <c r="E109" s="6" t="n"/>
       <c r="F109" s="6" t="n"/>
@@ -8924,7 +8924,7 @@
           <t>uri</t>
         </is>
       </c>
-      <c r="C159" s="6" t="inlineStr"/>
+      <c r="C159" s="6" t="n"/>
       <c r="D159" s="6" t="n"/>
       <c r="E159" s="6" t="n"/>
       <c r="F159" s="6" t="n"/>
@@ -11157,7 +11157,7 @@
       <c r="A222" s="4" t="inlineStr"/>
       <c r="B222" s="5" t="inlineStr">
         <is>
-          <t>code</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C222" s="6" t="n"/>
@@ -11193,7 +11193,7 @@
       <c r="A223" s="4" t="inlineStr"/>
       <c r="B223" s="5" t="inlineStr">
         <is>
-          <t>label</t>
+          <t>code</t>
         </is>
       </c>
       <c r="C223" s="6" t="n"/>
@@ -11229,7 +11229,7 @@
       <c r="A224" s="4" t="inlineStr"/>
       <c r="B224" s="5" t="inlineStr">
         <is>
-          <t>uri</t>
+          <t>label</t>
         </is>
       </c>
       <c r="C224" s="6" t="n"/>
@@ -11265,7 +11265,7 @@
       <c r="A225" s="4" t="inlineStr"/>
       <c r="B225" s="5" t="inlineStr">
         <is>
-          <t>relationship</t>
+          <t>uri</t>
         </is>
       </c>
       <c r="C225" s="6" t="n"/>
@@ -11301,7 +11301,7 @@
       <c r="A226" s="4" t="inlineStr"/>
       <c r="B226" s="5" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>relationship</t>
         </is>
       </c>
       <c r="C226" s="6" t="n"/>
@@ -11334,44 +11334,44 @@
       <c r="AD226" s="6" t="n"/>
     </row>
     <row r="227">
-      <c r="A227" s="4" t="n"/>
-      <c r="B227" s="8" t="n"/>
-      <c r="C227" s="2" t="n"/>
-      <c r="D227" s="2" t="n"/>
-      <c r="E227" s="2" t="n"/>
-      <c r="F227" s="2" t="n"/>
-      <c r="G227" s="2" t="n"/>
-      <c r="H227" s="2" t="n"/>
-      <c r="I227" s="2" t="n"/>
-      <c r="J227" s="2" t="n"/>
-      <c r="K227" s="2" t="n"/>
-      <c r="L227" s="2" t="n"/>
-      <c r="M227" s="2" t="n"/>
-      <c r="N227" s="2" t="n"/>
-      <c r="O227" s="2" t="n"/>
-      <c r="P227" s="2" t="n"/>
-      <c r="Q227" s="2" t="n"/>
-      <c r="R227" s="2" t="n"/>
-      <c r="S227" s="2" t="n"/>
-      <c r="T227" s="2" t="n"/>
-      <c r="U227" s="2" t="n"/>
-      <c r="V227" s="2" t="n"/>
-      <c r="W227" s="2" t="n"/>
-      <c r="X227" s="2" t="n"/>
-      <c r="Y227" s="2" t="n"/>
-      <c r="Z227" s="2" t="n"/>
-      <c r="AA227" s="2" t="n"/>
-      <c r="AB227" s="2" t="n"/>
-      <c r="AC227" s="2" t="n"/>
-      <c r="AD227" s="2" t="n"/>
+      <c r="A227" s="4" t="inlineStr"/>
+      <c r="B227" s="5" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C227" s="6" t="n"/>
+      <c r="D227" s="6" t="n"/>
+      <c r="E227" s="6" t="n"/>
+      <c r="F227" s="6" t="n"/>
+      <c r="G227" s="6" t="n"/>
+      <c r="H227" s="6" t="n"/>
+      <c r="I227" s="6" t="n"/>
+      <c r="J227" s="6" t="n"/>
+      <c r="K227" s="6" t="n"/>
+      <c r="L227" s="6" t="n"/>
+      <c r="M227" s="6" t="n"/>
+      <c r="N227" s="6" t="n"/>
+      <c r="O227" s="6" t="n"/>
+      <c r="P227" s="6" t="n"/>
+      <c r="Q227" s="6" t="n"/>
+      <c r="R227" s="6" t="n"/>
+      <c r="S227" s="6" t="n"/>
+      <c r="T227" s="6" t="n"/>
+      <c r="U227" s="6" t="n"/>
+      <c r="V227" s="6" t="n"/>
+      <c r="W227" s="6" t="n"/>
+      <c r="X227" s="6" t="n"/>
+      <c r="Y227" s="6" t="n"/>
+      <c r="Z227" s="6" t="n"/>
+      <c r="AA227" s="6" t="n"/>
+      <c r="AB227" s="6" t="n"/>
+      <c r="AC227" s="6" t="n"/>
+      <c r="AD227" s="6" t="n"/>
     </row>
     <row r="228">
-      <c r="A228" s="10" t="inlineStr">
-        <is>
-          <t>compliance</t>
-        </is>
-      </c>
-      <c r="B228" s="2" t="n"/>
+      <c r="A228" s="4" t="n"/>
+      <c r="B228" s="8" t="n"/>
       <c r="C228" s="2" t="n"/>
       <c r="D228" s="2" t="n"/>
       <c r="E228" s="2" t="n"/>
@@ -11402,49 +11402,49 @@
       <c r="AD228" s="2" t="n"/>
     </row>
     <row r="229">
-      <c r="A229" s="4" t="inlineStr"/>
-      <c r="B229" s="5" t="inlineStr">
-        <is>
-          <t>standard</t>
-        </is>
-      </c>
-      <c r="C229" s="6" t="inlineStr"/>
-      <c r="D229" s="6" t="n"/>
-      <c r="E229" s="6" t="n"/>
-      <c r="F229" s="6" t="n"/>
-      <c r="G229" s="6" t="n"/>
-      <c r="H229" s="6" t="n"/>
-      <c r="I229" s="6" t="n"/>
-      <c r="J229" s="6" t="n"/>
-      <c r="K229" s="6" t="n"/>
-      <c r="L229" s="6" t="n"/>
-      <c r="M229" s="6" t="n"/>
-      <c r="N229" s="6" t="n"/>
-      <c r="O229" s="6" t="n"/>
-      <c r="P229" s="6" t="n"/>
-      <c r="Q229" s="6" t="n"/>
-      <c r="R229" s="6" t="n"/>
-      <c r="S229" s="6" t="n"/>
-      <c r="T229" s="6" t="n"/>
-      <c r="U229" s="6" t="n"/>
-      <c r="V229" s="6" t="n"/>
-      <c r="W229" s="6" t="n"/>
-      <c r="X229" s="6" t="n"/>
-      <c r="Y229" s="6" t="n"/>
-      <c r="Z229" s="6" t="n"/>
-      <c r="AA229" s="6" t="n"/>
-      <c r="AB229" s="6" t="n"/>
-      <c r="AC229" s="6" t="n"/>
-      <c r="AD229" s="6" t="n"/>
+      <c r="A229" s="10" t="inlineStr">
+        <is>
+          <t>compliance</t>
+        </is>
+      </c>
+      <c r="B229" s="2" t="n"/>
+      <c r="C229" s="2" t="n"/>
+      <c r="D229" s="2" t="n"/>
+      <c r="E229" s="2" t="n"/>
+      <c r="F229" s="2" t="n"/>
+      <c r="G229" s="2" t="n"/>
+      <c r="H229" s="2" t="n"/>
+      <c r="I229" s="2" t="n"/>
+      <c r="J229" s="2" t="n"/>
+      <c r="K229" s="2" t="n"/>
+      <c r="L229" s="2" t="n"/>
+      <c r="M229" s="2" t="n"/>
+      <c r="N229" s="2" t="n"/>
+      <c r="O229" s="2" t="n"/>
+      <c r="P229" s="2" t="n"/>
+      <c r="Q229" s="2" t="n"/>
+      <c r="R229" s="2" t="n"/>
+      <c r="S229" s="2" t="n"/>
+      <c r="T229" s="2" t="n"/>
+      <c r="U229" s="2" t="n"/>
+      <c r="V229" s="2" t="n"/>
+      <c r="W229" s="2" t="n"/>
+      <c r="X229" s="2" t="n"/>
+      <c r="Y229" s="2" t="n"/>
+      <c r="Z229" s="2" t="n"/>
+      <c r="AA229" s="2" t="n"/>
+      <c r="AB229" s="2" t="n"/>
+      <c r="AC229" s="2" t="n"/>
+      <c r="AD229" s="2" t="n"/>
     </row>
     <row r="230">
       <c r="A230" s="4" t="inlineStr"/>
       <c r="B230" s="5" t="inlineStr">
         <is>
-          <t>abbreviation</t>
-        </is>
-      </c>
-      <c r="C230" s="6" t="n"/>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="C230" s="6" t="inlineStr"/>
       <c r="D230" s="6" t="n"/>
       <c r="E230" s="6" t="n"/>
       <c r="F230" s="6" t="n"/>
@@ -11477,7 +11477,7 @@
       <c r="A231" s="4" t="inlineStr"/>
       <c r="B231" s="5" t="inlineStr">
         <is>
-          <t>custodian</t>
+          <t>abbreviation</t>
         </is>
       </c>
       <c r="C231" s="6" t="n"/>
@@ -11513,7 +11513,7 @@
       <c r="A232" s="4" t="inlineStr"/>
       <c r="B232" s="5" t="inlineStr">
         <is>
-          <t>uri</t>
+          <t>custodian</t>
         </is>
       </c>
       <c r="C232" s="6" t="n"/>
@@ -11546,44 +11546,44 @@
       <c r="AD232" s="6" t="n"/>
     </row>
     <row r="233">
-      <c r="A233" s="4" t="n"/>
-      <c r="B233" s="8" t="n"/>
-      <c r="C233" s="2" t="n"/>
-      <c r="D233" s="2" t="n"/>
-      <c r="E233" s="2" t="n"/>
-      <c r="F233" s="2" t="n"/>
-      <c r="G233" s="2" t="n"/>
-      <c r="H233" s="2" t="n"/>
-      <c r="I233" s="2" t="n"/>
-      <c r="J233" s="2" t="n"/>
-      <c r="K233" s="2" t="n"/>
-      <c r="L233" s="2" t="n"/>
-      <c r="M233" s="2" t="n"/>
-      <c r="N233" s="2" t="n"/>
-      <c r="O233" s="2" t="n"/>
-      <c r="P233" s="2" t="n"/>
-      <c r="Q233" s="2" t="n"/>
-      <c r="R233" s="2" t="n"/>
-      <c r="S233" s="2" t="n"/>
-      <c r="T233" s="2" t="n"/>
-      <c r="U233" s="2" t="n"/>
-      <c r="V233" s="2" t="n"/>
-      <c r="W233" s="2" t="n"/>
-      <c r="X233" s="2" t="n"/>
-      <c r="Y233" s="2" t="n"/>
-      <c r="Z233" s="2" t="n"/>
-      <c r="AA233" s="2" t="n"/>
-      <c r="AB233" s="2" t="n"/>
-      <c r="AC233" s="2" t="n"/>
-      <c r="AD233" s="2" t="n"/>
+      <c r="A233" s="4" t="inlineStr"/>
+      <c r="B233" s="5" t="inlineStr">
+        <is>
+          <t>uri</t>
+        </is>
+      </c>
+      <c r="C233" s="6" t="n"/>
+      <c r="D233" s="6" t="n"/>
+      <c r="E233" s="6" t="n"/>
+      <c r="F233" s="6" t="n"/>
+      <c r="G233" s="6" t="n"/>
+      <c r="H233" s="6" t="n"/>
+      <c r="I233" s="6" t="n"/>
+      <c r="J233" s="6" t="n"/>
+      <c r="K233" s="6" t="n"/>
+      <c r="L233" s="6" t="n"/>
+      <c r="M233" s="6" t="n"/>
+      <c r="N233" s="6" t="n"/>
+      <c r="O233" s="6" t="n"/>
+      <c r="P233" s="6" t="n"/>
+      <c r="Q233" s="6" t="n"/>
+      <c r="R233" s="6" t="n"/>
+      <c r="S233" s="6" t="n"/>
+      <c r="T233" s="6" t="n"/>
+      <c r="U233" s="6" t="n"/>
+      <c r="V233" s="6" t="n"/>
+      <c r="W233" s="6" t="n"/>
+      <c r="X233" s="6" t="n"/>
+      <c r="Y233" s="6" t="n"/>
+      <c r="Z233" s="6" t="n"/>
+      <c r="AA233" s="6" t="n"/>
+      <c r="AB233" s="6" t="n"/>
+      <c r="AC233" s="6" t="n"/>
+      <c r="AD233" s="6" t="n"/>
     </row>
     <row r="234">
-      <c r="A234" s="10" t="inlineStr">
-        <is>
-          <t>framework</t>
-        </is>
-      </c>
-      <c r="B234" s="2" t="n"/>
+      <c r="A234" s="4" t="n"/>
+      <c r="B234" s="8" t="n"/>
       <c r="C234" s="2" t="n"/>
       <c r="D234" s="2" t="n"/>
       <c r="E234" s="2" t="n"/>
@@ -11614,49 +11614,49 @@
       <c r="AD234" s="2" t="n"/>
     </row>
     <row r="235">
-      <c r="A235" s="4" t="inlineStr"/>
-      <c r="B235" s="5" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C235" s="6" t="inlineStr"/>
-      <c r="D235" s="6" t="n"/>
-      <c r="E235" s="6" t="n"/>
-      <c r="F235" s="6" t="n"/>
-      <c r="G235" s="6" t="n"/>
-      <c r="H235" s="6" t="n"/>
-      <c r="I235" s="6" t="n"/>
-      <c r="J235" s="6" t="n"/>
-      <c r="K235" s="6" t="n"/>
-      <c r="L235" s="6" t="n"/>
-      <c r="M235" s="6" t="n"/>
-      <c r="N235" s="6" t="n"/>
-      <c r="O235" s="6" t="n"/>
-      <c r="P235" s="6" t="n"/>
-      <c r="Q235" s="6" t="n"/>
-      <c r="R235" s="6" t="n"/>
-      <c r="S235" s="6" t="n"/>
-      <c r="T235" s="6" t="n"/>
-      <c r="U235" s="6" t="n"/>
-      <c r="V235" s="6" t="n"/>
-      <c r="W235" s="6" t="n"/>
-      <c r="X235" s="6" t="n"/>
-      <c r="Y235" s="6" t="n"/>
-      <c r="Z235" s="6" t="n"/>
-      <c r="AA235" s="6" t="n"/>
-      <c r="AB235" s="6" t="n"/>
-      <c r="AC235" s="6" t="n"/>
-      <c r="AD235" s="6" t="n"/>
+      <c r="A235" s="10" t="inlineStr">
+        <is>
+          <t>framework</t>
+        </is>
+      </c>
+      <c r="B235" s="2" t="n"/>
+      <c r="C235" s="2" t="n"/>
+      <c r="D235" s="2" t="n"/>
+      <c r="E235" s="2" t="n"/>
+      <c r="F235" s="2" t="n"/>
+      <c r="G235" s="2" t="n"/>
+      <c r="H235" s="2" t="n"/>
+      <c r="I235" s="2" t="n"/>
+      <c r="J235" s="2" t="n"/>
+      <c r="K235" s="2" t="n"/>
+      <c r="L235" s="2" t="n"/>
+      <c r="M235" s="2" t="n"/>
+      <c r="N235" s="2" t="n"/>
+      <c r="O235" s="2" t="n"/>
+      <c r="P235" s="2" t="n"/>
+      <c r="Q235" s="2" t="n"/>
+      <c r="R235" s="2" t="n"/>
+      <c r="S235" s="2" t="n"/>
+      <c r="T235" s="2" t="n"/>
+      <c r="U235" s="2" t="n"/>
+      <c r="V235" s="2" t="n"/>
+      <c r="W235" s="2" t="n"/>
+      <c r="X235" s="2" t="n"/>
+      <c r="Y235" s="2" t="n"/>
+      <c r="Z235" s="2" t="n"/>
+      <c r="AA235" s="2" t="n"/>
+      <c r="AB235" s="2" t="n"/>
+      <c r="AC235" s="2" t="n"/>
+      <c r="AD235" s="2" t="n"/>
     </row>
     <row r="236">
       <c r="A236" s="4" t="inlineStr"/>
       <c r="B236" s="5" t="inlineStr">
         <is>
-          <t>abbreviation</t>
-        </is>
-      </c>
-      <c r="C236" s="6" t="n"/>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C236" s="6" t="inlineStr"/>
       <c r="D236" s="6" t="n"/>
       <c r="E236" s="6" t="n"/>
       <c r="F236" s="6" t="n"/>
@@ -11689,7 +11689,7 @@
       <c r="A237" s="4" t="inlineStr"/>
       <c r="B237" s="5" t="inlineStr">
         <is>
-          <t>custodian</t>
+          <t>abbreviation</t>
         </is>
       </c>
       <c r="C237" s="6" t="n"/>
@@ -11725,7 +11725,7 @@
       <c r="A238" s="4" t="inlineStr"/>
       <c r="B238" s="5" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>custodian</t>
         </is>
       </c>
       <c r="C238" s="6" t="n"/>
@@ -11761,7 +11761,7 @@
       <c r="A239" s="4" t="inlineStr"/>
       <c r="B239" s="5" t="inlineStr">
         <is>
-          <t>goal_id</t>
+          <t>description</t>
         </is>
       </c>
       <c r="C239" s="6" t="n"/>
@@ -11797,7 +11797,7 @@
       <c r="A240" s="4" t="inlineStr"/>
       <c r="B240" s="5" t="inlineStr">
         <is>
-          <t>goal_name</t>
+          <t>goal_id</t>
         </is>
       </c>
       <c r="C240" s="6" t="n"/>
@@ -11833,7 +11833,7 @@
       <c r="A241" s="4" t="inlineStr"/>
       <c r="B241" s="5" t="inlineStr">
         <is>
-          <t>goal_description</t>
+          <t>goal_name</t>
         </is>
       </c>
       <c r="C241" s="6" t="n"/>
@@ -11869,7 +11869,7 @@
       <c r="A242" s="4" t="inlineStr"/>
       <c r="B242" s="5" t="inlineStr">
         <is>
-          <t>target_id</t>
+          <t>goal_description</t>
         </is>
       </c>
       <c r="C242" s="6" t="n"/>
@@ -11905,7 +11905,7 @@
       <c r="A243" s="4" t="inlineStr"/>
       <c r="B243" s="5" t="inlineStr">
         <is>
-          <t>target_name</t>
+          <t>target_id</t>
         </is>
       </c>
       <c r="C243" s="6" t="n"/>
@@ -11941,7 +11941,7 @@
       <c r="A244" s="4" t="inlineStr"/>
       <c r="B244" s="5" t="inlineStr">
         <is>
-          <t>target_description</t>
+          <t>target_name</t>
         </is>
       </c>
       <c r="C244" s="6" t="n"/>
@@ -11977,7 +11977,7 @@
       <c r="A245" s="4" t="inlineStr"/>
       <c r="B245" s="5" t="inlineStr">
         <is>
-          <t>indicator_id</t>
+          <t>target_description</t>
         </is>
       </c>
       <c r="C245" s="6" t="n"/>
@@ -12013,7 +12013,7 @@
       <c r="A246" s="4" t="inlineStr"/>
       <c r="B246" s="5" t="inlineStr">
         <is>
-          <t>indicator_name</t>
+          <t>indicator_id</t>
         </is>
       </c>
       <c r="C246" s="6" t="n"/>
@@ -12049,7 +12049,7 @@
       <c r="A247" s="4" t="inlineStr"/>
       <c r="B247" s="5" t="inlineStr">
         <is>
-          <t>indicator_description</t>
+          <t>indicator_name</t>
         </is>
       </c>
       <c r="C247" s="6" t="n"/>
@@ -12085,7 +12085,7 @@
       <c r="A248" s="4" t="inlineStr"/>
       <c r="B248" s="5" t="inlineStr">
         <is>
-          <t>uri</t>
+          <t>indicator_description</t>
         </is>
       </c>
       <c r="C248" s="6" t="n"/>
@@ -12121,7 +12121,7 @@
       <c r="A249" s="4" t="inlineStr"/>
       <c r="B249" s="5" t="inlineStr">
         <is>
-          <t>notes</t>
+          <t>uri</t>
         </is>
       </c>
       <c r="C249" s="6" t="n"/>
@@ -12154,44 +12154,44 @@
       <c r="AD249" s="6" t="n"/>
     </row>
     <row r="250">
-      <c r="A250" s="4" t="n"/>
-      <c r="B250" s="8" t="n"/>
-      <c r="C250" s="2" t="n"/>
-      <c r="D250" s="2" t="n"/>
-      <c r="E250" s="2" t="n"/>
-      <c r="F250" s="2" t="n"/>
-      <c r="G250" s="2" t="n"/>
-      <c r="H250" s="2" t="n"/>
-      <c r="I250" s="2" t="n"/>
-      <c r="J250" s="2" t="n"/>
-      <c r="K250" s="2" t="n"/>
-      <c r="L250" s="2" t="n"/>
-      <c r="M250" s="2" t="n"/>
-      <c r="N250" s="2" t="n"/>
-      <c r="O250" s="2" t="n"/>
-      <c r="P250" s="2" t="n"/>
-      <c r="Q250" s="2" t="n"/>
-      <c r="R250" s="2" t="n"/>
-      <c r="S250" s="2" t="n"/>
-      <c r="T250" s="2" t="n"/>
-      <c r="U250" s="2" t="n"/>
-      <c r="V250" s="2" t="n"/>
-      <c r="W250" s="2" t="n"/>
-      <c r="X250" s="2" t="n"/>
-      <c r="Y250" s="2" t="n"/>
-      <c r="Z250" s="2" t="n"/>
-      <c r="AA250" s="2" t="n"/>
-      <c r="AB250" s="2" t="n"/>
-      <c r="AC250" s="2" t="n"/>
-      <c r="AD250" s="2" t="n"/>
+      <c r="A250" s="4" t="inlineStr"/>
+      <c r="B250" s="5" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="C250" s="6" t="n"/>
+      <c r="D250" s="6" t="n"/>
+      <c r="E250" s="6" t="n"/>
+      <c r="F250" s="6" t="n"/>
+      <c r="G250" s="6" t="n"/>
+      <c r="H250" s="6" t="n"/>
+      <c r="I250" s="6" t="n"/>
+      <c r="J250" s="6" t="n"/>
+      <c r="K250" s="6" t="n"/>
+      <c r="L250" s="6" t="n"/>
+      <c r="M250" s="6" t="n"/>
+      <c r="N250" s="6" t="n"/>
+      <c r="O250" s="6" t="n"/>
+      <c r="P250" s="6" t="n"/>
+      <c r="Q250" s="6" t="n"/>
+      <c r="R250" s="6" t="n"/>
+      <c r="S250" s="6" t="n"/>
+      <c r="T250" s="6" t="n"/>
+      <c r="U250" s="6" t="n"/>
+      <c r="V250" s="6" t="n"/>
+      <c r="W250" s="6" t="n"/>
+      <c r="X250" s="6" t="n"/>
+      <c r="Y250" s="6" t="n"/>
+      <c r="Z250" s="6" t="n"/>
+      <c r="AA250" s="6" t="n"/>
+      <c r="AB250" s="6" t="n"/>
+      <c r="AC250" s="6" t="n"/>
+      <c r="AD250" s="6" t="n"/>
     </row>
     <row r="251">
-      <c r="A251" s="10" t="inlineStr">
-        <is>
-          <t>series_groups</t>
-        </is>
-      </c>
-      <c r="B251" s="2" t="n"/>
+      <c r="A251" s="4" t="n"/>
+      <c r="B251" s="8" t="n"/>
       <c r="C251" s="2" t="n"/>
       <c r="D251" s="2" t="n"/>
       <c r="E251" s="2" t="n"/>
@@ -12222,46 +12222,46 @@
       <c r="AD251" s="2" t="n"/>
     </row>
     <row r="252">
-      <c r="A252" s="4" t="inlineStr"/>
-      <c r="B252" s="5" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C252" s="6" t="n"/>
-      <c r="D252" s="6" t="n"/>
-      <c r="E252" s="6" t="n"/>
-      <c r="F252" s="6" t="n"/>
-      <c r="G252" s="6" t="n"/>
-      <c r="H252" s="6" t="n"/>
-      <c r="I252" s="6" t="n"/>
-      <c r="J252" s="6" t="n"/>
-      <c r="K252" s="6" t="n"/>
-      <c r="L252" s="6" t="n"/>
-      <c r="M252" s="6" t="n"/>
-      <c r="N252" s="6" t="n"/>
-      <c r="O252" s="6" t="n"/>
-      <c r="P252" s="6" t="n"/>
-      <c r="Q252" s="6" t="n"/>
-      <c r="R252" s="6" t="n"/>
-      <c r="S252" s="6" t="n"/>
-      <c r="T252" s="6" t="n"/>
-      <c r="U252" s="6" t="n"/>
-      <c r="V252" s="6" t="n"/>
-      <c r="W252" s="6" t="n"/>
-      <c r="X252" s="6" t="n"/>
-      <c r="Y252" s="6" t="n"/>
-      <c r="Z252" s="6" t="n"/>
-      <c r="AA252" s="6" t="n"/>
-      <c r="AB252" s="6" t="n"/>
-      <c r="AC252" s="6" t="n"/>
-      <c r="AD252" s="6" t="n"/>
+      <c r="A252" s="10" t="inlineStr">
+        <is>
+          <t>series_groups</t>
+        </is>
+      </c>
+      <c r="B252" s="2" t="n"/>
+      <c r="C252" s="2" t="n"/>
+      <c r="D252" s="2" t="n"/>
+      <c r="E252" s="2" t="n"/>
+      <c r="F252" s="2" t="n"/>
+      <c r="G252" s="2" t="n"/>
+      <c r="H252" s="2" t="n"/>
+      <c r="I252" s="2" t="n"/>
+      <c r="J252" s="2" t="n"/>
+      <c r="K252" s="2" t="n"/>
+      <c r="L252" s="2" t="n"/>
+      <c r="M252" s="2" t="n"/>
+      <c r="N252" s="2" t="n"/>
+      <c r="O252" s="2" t="n"/>
+      <c r="P252" s="2" t="n"/>
+      <c r="Q252" s="2" t="n"/>
+      <c r="R252" s="2" t="n"/>
+      <c r="S252" s="2" t="n"/>
+      <c r="T252" s="2" t="n"/>
+      <c r="U252" s="2" t="n"/>
+      <c r="V252" s="2" t="n"/>
+      <c r="W252" s="2" t="n"/>
+      <c r="X252" s="2" t="n"/>
+      <c r="Y252" s="2" t="n"/>
+      <c r="Z252" s="2" t="n"/>
+      <c r="AA252" s="2" t="n"/>
+      <c r="AB252" s="2" t="n"/>
+      <c r="AC252" s="2" t="n"/>
+      <c r="AD252" s="2" t="n"/>
     </row>
     <row r="253">
       <c r="A253" s="4" t="inlineStr"/>
       <c r="B253" s="5" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C253" s="6" t="n"/>
@@ -12297,7 +12297,7 @@
       <c r="A254" s="4" t="inlineStr"/>
       <c r="B254" s="5" t="inlineStr">
         <is>
-          <t>version</t>
+          <t>description</t>
         </is>
       </c>
       <c r="C254" s="6" t="n"/>
@@ -12333,7 +12333,7 @@
       <c r="A255" s="4" t="inlineStr"/>
       <c r="B255" s="5" t="inlineStr">
         <is>
-          <t>uri</t>
+          <t>version</t>
         </is>
       </c>
       <c r="C255" s="6" t="n"/>
@@ -12366,44 +12366,44 @@
       <c r="AD255" s="6" t="n"/>
     </row>
     <row r="256">
-      <c r="A256" s="4" t="n"/>
-      <c r="B256" s="8" t="n"/>
-      <c r="C256" s="2" t="n"/>
-      <c r="D256" s="2" t="n"/>
-      <c r="E256" s="2" t="n"/>
-      <c r="F256" s="2" t="n"/>
-      <c r="G256" s="2" t="n"/>
-      <c r="H256" s="2" t="n"/>
-      <c r="I256" s="2" t="n"/>
-      <c r="J256" s="2" t="n"/>
-      <c r="K256" s="2" t="n"/>
-      <c r="L256" s="2" t="n"/>
-      <c r="M256" s="2" t="n"/>
-      <c r="N256" s="2" t="n"/>
-      <c r="O256" s="2" t="n"/>
-      <c r="P256" s="2" t="n"/>
-      <c r="Q256" s="2" t="n"/>
-      <c r="R256" s="2" t="n"/>
-      <c r="S256" s="2" t="n"/>
-      <c r="T256" s="2" t="n"/>
-      <c r="U256" s="2" t="n"/>
-      <c r="V256" s="2" t="n"/>
-      <c r="W256" s="2" t="n"/>
-      <c r="X256" s="2" t="n"/>
-      <c r="Y256" s="2" t="n"/>
-      <c r="Z256" s="2" t="n"/>
-      <c r="AA256" s="2" t="n"/>
-      <c r="AB256" s="2" t="n"/>
-      <c r="AC256" s="2" t="n"/>
-      <c r="AD256" s="2" t="n"/>
+      <c r="A256" s="4" t="inlineStr"/>
+      <c r="B256" s="5" t="inlineStr">
+        <is>
+          <t>uri</t>
+        </is>
+      </c>
+      <c r="C256" s="6" t="n"/>
+      <c r="D256" s="6" t="n"/>
+      <c r="E256" s="6" t="n"/>
+      <c r="F256" s="6" t="n"/>
+      <c r="G256" s="6" t="n"/>
+      <c r="H256" s="6" t="n"/>
+      <c r="I256" s="6" t="n"/>
+      <c r="J256" s="6" t="n"/>
+      <c r="K256" s="6" t="n"/>
+      <c r="L256" s="6" t="n"/>
+      <c r="M256" s="6" t="n"/>
+      <c r="N256" s="6" t="n"/>
+      <c r="O256" s="6" t="n"/>
+      <c r="P256" s="6" t="n"/>
+      <c r="Q256" s="6" t="n"/>
+      <c r="R256" s="6" t="n"/>
+      <c r="S256" s="6" t="n"/>
+      <c r="T256" s="6" t="n"/>
+      <c r="U256" s="6" t="n"/>
+      <c r="V256" s="6" t="n"/>
+      <c r="W256" s="6" t="n"/>
+      <c r="X256" s="6" t="n"/>
+      <c r="Y256" s="6" t="n"/>
+      <c r="Z256" s="6" t="n"/>
+      <c r="AA256" s="6" t="n"/>
+      <c r="AB256" s="6" t="n"/>
+      <c r="AC256" s="6" t="n"/>
+      <c r="AD256" s="6" t="n"/>
     </row>
     <row r="257">
-      <c r="A257" s="10" t="inlineStr">
-        <is>
-          <t>contacts</t>
-        </is>
-      </c>
-      <c r="B257" s="2" t="n"/>
+      <c r="A257" s="4" t="n"/>
+      <c r="B257" s="8" t="n"/>
       <c r="C257" s="2" t="n"/>
       <c r="D257" s="2" t="n"/>
       <c r="E257" s="2" t="n"/>
@@ -12434,46 +12434,46 @@
       <c r="AD257" s="2" t="n"/>
     </row>
     <row r="258">
-      <c r="A258" s="4" t="inlineStr"/>
-      <c r="B258" s="5" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C258" s="6" t="n"/>
-      <c r="D258" s="6" t="n"/>
-      <c r="E258" s="6" t="n"/>
-      <c r="F258" s="6" t="n"/>
-      <c r="G258" s="6" t="n"/>
-      <c r="H258" s="6" t="n"/>
-      <c r="I258" s="6" t="n"/>
-      <c r="J258" s="6" t="n"/>
-      <c r="K258" s="6" t="n"/>
-      <c r="L258" s="6" t="n"/>
-      <c r="M258" s="6" t="n"/>
-      <c r="N258" s="6" t="n"/>
-      <c r="O258" s="6" t="n"/>
-      <c r="P258" s="6" t="n"/>
-      <c r="Q258" s="6" t="n"/>
-      <c r="R258" s="6" t="n"/>
-      <c r="S258" s="6" t="n"/>
-      <c r="T258" s="6" t="n"/>
-      <c r="U258" s="6" t="n"/>
-      <c r="V258" s="6" t="n"/>
-      <c r="W258" s="6" t="n"/>
-      <c r="X258" s="6" t="n"/>
-      <c r="Y258" s="6" t="n"/>
-      <c r="Z258" s="6" t="n"/>
-      <c r="AA258" s="6" t="n"/>
-      <c r="AB258" s="6" t="n"/>
-      <c r="AC258" s="6" t="n"/>
-      <c r="AD258" s="6" t="n"/>
+      <c r="A258" s="10" t="inlineStr">
+        <is>
+          <t>contacts</t>
+        </is>
+      </c>
+      <c r="B258" s="2" t="n"/>
+      <c r="C258" s="2" t="n"/>
+      <c r="D258" s="2" t="n"/>
+      <c r="E258" s="2" t="n"/>
+      <c r="F258" s="2" t="n"/>
+      <c r="G258" s="2" t="n"/>
+      <c r="H258" s="2" t="n"/>
+      <c r="I258" s="2" t="n"/>
+      <c r="J258" s="2" t="n"/>
+      <c r="K258" s="2" t="n"/>
+      <c r="L258" s="2" t="n"/>
+      <c r="M258" s="2" t="n"/>
+      <c r="N258" s="2" t="n"/>
+      <c r="O258" s="2" t="n"/>
+      <c r="P258" s="2" t="n"/>
+      <c r="Q258" s="2" t="n"/>
+      <c r="R258" s="2" t="n"/>
+      <c r="S258" s="2" t="n"/>
+      <c r="T258" s="2" t="n"/>
+      <c r="U258" s="2" t="n"/>
+      <c r="V258" s="2" t="n"/>
+      <c r="W258" s="2" t="n"/>
+      <c r="X258" s="2" t="n"/>
+      <c r="Y258" s="2" t="n"/>
+      <c r="Z258" s="2" t="n"/>
+      <c r="AA258" s="2" t="n"/>
+      <c r="AB258" s="2" t="n"/>
+      <c r="AC258" s="2" t="n"/>
+      <c r="AD258" s="2" t="n"/>
     </row>
     <row r="259">
       <c r="A259" s="4" t="inlineStr"/>
       <c r="B259" s="5" t="inlineStr">
         <is>
-          <t>role</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C259" s="6" t="n"/>
@@ -12509,7 +12509,7 @@
       <c r="A260" s="4" t="inlineStr"/>
       <c r="B260" s="5" t="inlineStr">
         <is>
-          <t>position</t>
+          <t>role</t>
         </is>
       </c>
       <c r="C260" s="6" t="n"/>
@@ -12545,7 +12545,7 @@
       <c r="A261" s="4" t="inlineStr"/>
       <c r="B261" s="5" t="inlineStr">
         <is>
-          <t>affiliation</t>
+          <t>position</t>
         </is>
       </c>
       <c r="C261" s="6" t="n"/>
@@ -12581,7 +12581,7 @@
       <c r="A262" s="4" t="inlineStr"/>
       <c r="B262" s="5" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>affiliation</t>
         </is>
       </c>
       <c r="C262" s="6" t="n"/>
@@ -12617,7 +12617,7 @@
       <c r="A263" s="4" t="inlineStr"/>
       <c r="B263" s="5" t="inlineStr">
         <is>
-          <t>telephone</t>
+          <t>email</t>
         </is>
       </c>
       <c r="C263" s="6" t="n"/>
@@ -12653,7 +12653,7 @@
       <c r="A264" s="4" t="inlineStr"/>
       <c r="B264" s="5" t="inlineStr">
         <is>
-          <t>uri</t>
+          <t>telephone</t>
         </is>
       </c>
       <c r="C264" s="6" t="n"/>
@@ -12686,68 +12686,72 @@
       <c r="AD264" s="6" t="n"/>
     </row>
     <row r="265">
-      <c r="A265" s="4" t="n"/>
-      <c r="B265" s="8" t="n"/>
-      <c r="C265" s="2" t="n"/>
-      <c r="D265" s="2" t="n"/>
-      <c r="E265" s="2" t="n"/>
-      <c r="F265" s="2" t="n"/>
-      <c r="G265" s="2" t="n"/>
-      <c r="H265" s="2" t="n"/>
-      <c r="I265" s="2" t="n"/>
-      <c r="J265" s="2" t="n"/>
-      <c r="K265" s="2" t="n"/>
-      <c r="L265" s="2" t="n"/>
-      <c r="M265" s="2" t="n"/>
-      <c r="N265" s="2" t="n"/>
-      <c r="O265" s="2" t="n"/>
-      <c r="P265" s="2" t="n"/>
-      <c r="Q265" s="2" t="n"/>
-      <c r="R265" s="2" t="n"/>
-      <c r="S265" s="2" t="n"/>
-      <c r="T265" s="2" t="n"/>
-      <c r="U265" s="2" t="n"/>
-      <c r="V265" s="2" t="n"/>
-      <c r="W265" s="2" t="n"/>
-      <c r="X265" s="2" t="n"/>
-      <c r="Y265" s="2" t="n"/>
-      <c r="Z265" s="2" t="n"/>
-      <c r="AA265" s="2" t="n"/>
-      <c r="AB265" s="2" t="n"/>
-      <c r="AC265" s="2" t="n"/>
-      <c r="AD265" s="2" t="n"/>
+      <c r="A265" s="4" t="inlineStr"/>
+      <c r="B265" s="5" t="inlineStr">
+        <is>
+          <t>uri</t>
+        </is>
+      </c>
+      <c r="C265" s="6" t="n"/>
+      <c r="D265" s="6" t="n"/>
+      <c r="E265" s="6" t="n"/>
+      <c r="F265" s="6" t="n"/>
+      <c r="G265" s="6" t="n"/>
+      <c r="H265" s="6" t="n"/>
+      <c r="I265" s="6" t="n"/>
+      <c r="J265" s="6" t="n"/>
+      <c r="K265" s="6" t="n"/>
+      <c r="L265" s="6" t="n"/>
+      <c r="M265" s="6" t="n"/>
+      <c r="N265" s="6" t="n"/>
+      <c r="O265" s="6" t="n"/>
+      <c r="P265" s="6" t="n"/>
+      <c r="Q265" s="6" t="n"/>
+      <c r="R265" s="6" t="n"/>
+      <c r="S265" s="6" t="n"/>
+      <c r="T265" s="6" t="n"/>
+      <c r="U265" s="6" t="n"/>
+      <c r="V265" s="6" t="n"/>
+      <c r="W265" s="6" t="n"/>
+      <c r="X265" s="6" t="n"/>
+      <c r="Y265" s="6" t="n"/>
+      <c r="Z265" s="6" t="n"/>
+      <c r="AA265" s="6" t="n"/>
+      <c r="AB265" s="6" t="n"/>
+      <c r="AC265" s="6" t="n"/>
+      <c r="AD265" s="6" t="n"/>
     </row>
     <row r="266">
       <c r="A266" s="4" t="n"/>
-      <c r="B266" s="4" t="n"/>
-      <c r="C266" s="4" t="n"/>
-      <c r="D266" s="4" t="n"/>
-      <c r="E266" s="4" t="n"/>
-      <c r="F266" s="4" t="n"/>
-      <c r="G266" s="4" t="n"/>
-      <c r="H266" s="4" t="n"/>
-      <c r="I266" s="4" t="n"/>
-      <c r="J266" s="4" t="n"/>
-      <c r="K266" s="4" t="n"/>
-      <c r="L266" s="4" t="n"/>
-      <c r="M266" s="4" t="n"/>
-      <c r="N266" s="4" t="n"/>
-      <c r="O266" s="4" t="n"/>
-      <c r="P266" s="4" t="n"/>
-      <c r="Q266" s="4" t="n"/>
-      <c r="R266" s="4" t="n"/>
-      <c r="S266" s="4" t="n"/>
-      <c r="T266" s="4" t="n"/>
-      <c r="U266" s="4" t="n"/>
-      <c r="V266" s="4" t="n"/>
-      <c r="W266" s="4" t="n"/>
-      <c r="X266" s="4" t="n"/>
-      <c r="Y266" s="4" t="n"/>
-      <c r="Z266" s="4" t="n"/>
-      <c r="AA266" s="4" t="n"/>
-      <c r="AB266" s="4" t="n"/>
-      <c r="AC266" s="4" t="n"/>
-      <c r="AD266" s="4" t="n"/>
+      <c r="B266" s="8" t="n"/>
+      <c r="C266" s="2" t="n"/>
+      <c r="D266" s="2" t="n"/>
+      <c r="E266" s="2" t="n"/>
+      <c r="F266" s="2" t="n"/>
+      <c r="G266" s="2" t="n"/>
+      <c r="H266" s="2" t="n"/>
+      <c r="I266" s="2" t="n"/>
+      <c r="J266" s="2" t="n"/>
+      <c r="K266" s="2" t="n"/>
+      <c r="L266" s="2" t="n"/>
+      <c r="M266" s="2" t="n"/>
+      <c r="N266" s="2" t="n"/>
+      <c r="O266" s="2" t="n"/>
+      <c r="P266" s="2" t="n"/>
+      <c r="Q266" s="2" t="n"/>
+      <c r="R266" s="2" t="n"/>
+      <c r="S266" s="2" t="n"/>
+      <c r="T266" s="2" t="n"/>
+      <c r="U266" s="2" t="n"/>
+      <c r="V266" s="2" t="n"/>
+      <c r="W266" s="2" t="n"/>
+      <c r="X266" s="2" t="n"/>
+      <c r="Y266" s="2" t="n"/>
+      <c r="Z266" s="2" t="n"/>
+      <c r="AA266" s="2" t="n"/>
+      <c r="AB266" s="2" t="n"/>
+      <c r="AC266" s="2" t="n"/>
+      <c r="AD266" s="2" t="n"/>
     </row>
     <row r="267">
       <c r="A267" s="4" t="n"/>
@@ -13677,6 +13681,38 @@
       <c r="AC295" s="4" t="n"/>
       <c r="AD295" s="4" t="n"/>
     </row>
+    <row r="296">
+      <c r="A296" s="4" t="n"/>
+      <c r="B296" s="4" t="n"/>
+      <c r="C296" s="4" t="n"/>
+      <c r="D296" s="4" t="n"/>
+      <c r="E296" s="4" t="n"/>
+      <c r="F296" s="4" t="n"/>
+      <c r="G296" s="4" t="n"/>
+      <c r="H296" s="4" t="n"/>
+      <c r="I296" s="4" t="n"/>
+      <c r="J296" s="4" t="n"/>
+      <c r="K296" s="4" t="n"/>
+      <c r="L296" s="4" t="n"/>
+      <c r="M296" s="4" t="n"/>
+      <c r="N296" s="4" t="n"/>
+      <c r="O296" s="4" t="n"/>
+      <c r="P296" s="4" t="n"/>
+      <c r="Q296" s="4" t="n"/>
+      <c r="R296" s="4" t="n"/>
+      <c r="S296" s="4" t="n"/>
+      <c r="T296" s="4" t="n"/>
+      <c r="U296" s="4" t="n"/>
+      <c r="V296" s="4" t="n"/>
+      <c r="W296" s="4" t="n"/>
+      <c r="X296" s="4" t="n"/>
+      <c r="Y296" s="4" t="n"/>
+      <c r="Z296" s="4" t="n"/>
+      <c r="AA296" s="4" t="n"/>
+      <c r="AB296" s="4" t="n"/>
+      <c r="AC296" s="4" t="n"/>
+      <c r="AD296" s="4" t="n"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="0" autoFilter="1" scenarios="0" formatColumns="0" deleteColumns="0" insertColumns="0" pivotTables="1" deleteRows="1" formatCells="0" formatRows="0" sort="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13979,7 +14015,7 @@
       </c>
       <c r="D8" s="6" t="inlineStr">
         <is>
-          <t>[{"code": null, "name": null, "description": null}]</t>
+          <t>[{"code": null, "label": null, "description": null}]</t>
         </is>
       </c>
       <c r="E8" s="6" t="n"/>

</xml_diff>